<commit_message>
adding pdbbind dataset and jupyter notebook
</commit_message>
<xml_diff>
--- a/Results/host-guest-dataset_clean.xlsx
+++ b/Results/host-guest-dataset_clean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/misspotato/Documents/GitHub/Host-Guest System gbnsr6/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/misspotato/Documents/GitHub/Binding-Free-Energy-Prediction-Host-Guest-System/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E68A5F-45B0-EF4D-996F-370C2997D63E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEFB308-B6D8-AC40-9D62-92921F51639B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="-18380" windowWidth="31140" windowHeight="16740" activeTab="1" xr2:uid="{B5BBD327-6A3B-EE47-875C-25D1AD5D16D6}"/>
+    <workbookView xWindow="700" yWindow="-18460" windowWidth="34080" windowHeight="16740" xr2:uid="{B5BBD327-6A3B-EE47-875C-25D1AD5D16D6}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
+    <pivotCache cacheId="24" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="93">
   <si>
     <t>dataset group name</t>
   </si>
@@ -298,24 +298,6 @@
     <t>With istrng=0</t>
   </si>
   <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
-    <t>G5</t>
-  </si>
-  <si>
-    <t>G6</t>
-  </si>
-  <si>
     <t>SAMPL5</t>
   </si>
   <si>
@@ -323,6 +305,9 @@
   </si>
   <si>
     <t>OAME</t>
+  </si>
+  <si>
+    <t>sample</t>
   </si>
 </sst>
 </file>
@@ -7724,7 +7709,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{041C620A-01CB-D248-AD5D-9E58A9EA1194}" name="PivotTable6" cacheId="13" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{041C620A-01CB-D248-AD5D-9E58A9EA1194}" name="PivotTable6" cacheId="24" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:D63" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0">
@@ -8507,10 +8492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCD74DF-FB71-A641-B99D-0471020535CD}">
-  <dimension ref="A1:AS63"/>
+  <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AE1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8560,7 +8545,10 @@
     <col min="43" max="43" width="20" style="4" customWidth="1"/>
     <col min="44" max="44" width="25" style="4" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="18.83203125" style="4" customWidth="1"/>
-    <col min="46" max="16384" width="10.83203125" style="4"/>
+    <col min="46" max="47" width="10.83203125" style="4"/>
+    <col min="48" max="48" width="17.83203125" style="4" customWidth="1"/>
+    <col min="49" max="49" width="17.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -13363,18 +13351,18 @@
         <v>5.9691999999999998</v>
       </c>
       <c r="AN34" s="6">
-        <f t="shared" ref="AN34:AN63" si="5">(Y34+U34)-((AD34+K34)+(AI34+P34))</f>
+        <f t="shared" ref="AN34:AN68" si="5">(Y34+U34)-((AD34+K34)+(AI34+P34))</f>
         <v>-8.0108999999999924</v>
       </c>
       <c r="AO34" s="4">
-        <f t="shared" ref="AO34:AO63" si="6">T34-(O34+J34)</f>
+        <f t="shared" ref="AO34:AO68" si="6">T34-(O34+J34)</f>
         <v>-8.0243000000000393</v>
       </c>
       <c r="AP34" s="6">
         <v>-1.96</v>
       </c>
       <c r="AQ34" s="4">
-        <f t="shared" ref="AQ34:AQ63" si="7">AN34-AP34</f>
+        <f t="shared" ref="AQ34:AQ68" si="7">AN34-AP34</f>
         <v>-6.0508999999999924</v>
       </c>
       <c r="AR34" s="4">
@@ -16231,13 +16219,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="F55" s="4">
         <v>-5.04</v>
@@ -16370,13 +16361,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="F56" s="4">
         <v>-4.25</v>
@@ -16509,13 +16503,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="F57" s="4">
         <v>-5.0599999999999996</v>
@@ -16648,13 +16645,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="F58" s="4">
         <v>-9.3699999999999992</v>
@@ -16787,13 +16787,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="F59" s="4">
         <v>-4.5</v>
@@ -16926,13 +16929,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="F60" s="4">
         <v>-5.33</v>
@@ -17065,13 +17071,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="F61" s="4">
         <v>-5.24</v>
@@ -17204,13 +17213,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="F62" s="4">
         <v>-5.04</v>
@@ -17343,13 +17355,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="F63" s="4">
         <v>-4.5199999999999996</v>
@@ -17476,6 +17491,21 @@
         <f t="shared" si="9"/>
         <v>4.5672000000000033</v>
       </c>
+    </row>
+    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AN64" s="6"/>
+    </row>
+    <row r="65" spans="40:40" x14ac:dyDescent="0.2">
+      <c r="AN65" s="6"/>
+    </row>
+    <row r="66" spans="40:40" x14ac:dyDescent="0.2">
+      <c r="AN66" s="6"/>
+    </row>
+    <row r="67" spans="40:40" x14ac:dyDescent="0.2">
+      <c r="AN67" s="6"/>
+    </row>
+    <row r="68" spans="40:40" x14ac:dyDescent="0.2">
+      <c r="AN68" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17486,8 +17516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA4B728-D30D-F64A-A693-296E63233403}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH20" sqref="AH20"/>
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>